<commit_message>
Update Test Case: Template (1)
</commit_message>
<xml_diff>
--- a/System 6 Renovation Working Files/Test Files/Template (1).xlsx
+++ b/System 6 Renovation Working Files/Test Files/Template (1).xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19020" windowHeight="8325"/>
   </bookViews>
@@ -968,6 +968,24 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="63" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="66" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="66" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="45" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -991,24 +1009,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="63" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="66" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="66" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1379,10 +1379,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1394,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2">
@@ -1404,7 +1405,7 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="32"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="2">
         <v>7</v>
       </c>
@@ -1413,7 +1414,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="39" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5">
@@ -1424,7 +1425,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="4">
         <v>4</v>
       </c>
@@ -1433,7 +1434,7 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="4">
         <v>5</v>
       </c>
@@ -1442,7 +1443,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="4">
         <v>6</v>
       </c>
@@ -1451,7 +1452,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="4">
         <v>7</v>
       </c>
@@ -1471,7 +1472,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="10">
@@ -1482,7 +1483,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="9">
         <v>4</v>
       </c>
@@ -1491,7 +1492,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="9">
         <v>5</v>
       </c>
@@ -1500,7 +1501,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="9">
         <v>6</v>
       </c>
@@ -1509,7 +1510,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="9">
         <v>7</v>
       </c>
@@ -1518,7 +1519,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="10">
         <v>8</v>
       </c>
@@ -1527,7 +1528,7 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="41" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="15">
@@ -1538,7 +1539,7 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="15">
         <v>3</v>
       </c>
@@ -1547,7 +1548,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="45" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="17">
@@ -1558,7 +1559,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="17">
         <v>3</v>
       </c>
@@ -1578,7 +1579,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="45" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="17">
@@ -1589,7 +1590,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="17">
         <v>3</v>
       </c>
@@ -1598,7 +1599,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="45" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="17">
@@ -1609,7 +1610,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="17">
         <v>3</v>
       </c>
@@ -1618,10 +1619,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="20">
@@ -1632,8 +1633,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="40"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="20">
         <v>4</v>
       </c>
@@ -1642,8 +1643,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="40"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="19">
         <v>5</v>
       </c>
@@ -1652,8 +1653,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="40"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="19">
         <v>8</v>
       </c>
@@ -1662,8 +1663,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="40"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="19">
         <v>10</v>
       </c>
@@ -1672,8 +1673,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="19">
         <v>12</v>
       </c>
@@ -1682,8 +1683,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="19">
         <v>13</v>
       </c>
@@ -1692,8 +1693,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="19">
         <v>14</v>
       </c>
@@ -1702,8 +1703,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="19">
         <v>15</v>
       </c>
@@ -1712,8 +1713,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="33"/>
+      <c r="B33" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="20">
@@ -1724,8 +1725,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="19">
         <v>4</v>
       </c>
@@ -1734,8 +1735,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="19">
         <v>5</v>
       </c>
@@ -1744,8 +1745,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="40"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="19">
         <v>6</v>
       </c>
@@ -1754,8 +1755,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="20">
         <v>7</v>
       </c>
@@ -1764,8 +1765,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="19">
         <v>8</v>
       </c>
@@ -1774,8 +1775,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="19">
         <v>10</v>
       </c>
@@ -1784,8 +1785,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="19">
         <v>11</v>
       </c>
@@ -1794,8 +1795,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="35"/>
       <c r="C41" s="19">
         <v>12</v>
       </c>
@@ -1804,8 +1805,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="40"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="19">
         <v>14</v>
       </c>
@@ -1814,7 +1815,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="25" t="s">
         <v>64</v>
       </c>
@@ -1826,8 +1827,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="40" t="s">
+      <c r="A44" s="33"/>
+      <c r="B44" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C44" s="19">
@@ -1838,8 +1839,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="19">
         <v>4</v>
       </c>
@@ -1848,8 +1849,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="19">
         <v>5</v>
       </c>
@@ -1858,8 +1859,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="40"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="19">
         <v>8</v>
       </c>
@@ -1868,8 +1869,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="40"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="35"/>
       <c r="C48" s="19">
         <v>9</v>
       </c>
@@ -1878,8 +1879,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="40"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="35"/>
       <c r="C49" s="19">
         <v>10</v>
       </c>
@@ -1888,124 +1889,124 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="36" t="s">
+      <c r="A50" s="33"/>
+      <c r="B50" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="17">
+        <v>3</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="33"/>
+      <c r="B51" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="13">
+      <c r="C51" s="13">
         <v>4</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D51" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="13">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="33"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="13">
         <v>5</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="12">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="33"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="12">
         <v>6</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="12">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="33"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="12">
         <v>7</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D54" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="12">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="12">
         <v>8</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="12">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="33"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="12">
         <v>9</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="12">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="12">
         <v>10</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="12">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="33"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="12">
         <v>12</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D58" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="12">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="33"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="12">
         <v>14</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D59" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="12">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="34"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="12">
         <v>15</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="45"/>
-      <c r="B60" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C60" s="17">
-        <v>3</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B61" s="40" t="s">
+      <c r="B61" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C61" s="20">
@@ -2016,8 +2017,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="40"/>
+      <c r="A62" s="33"/>
+      <c r="B62" s="35"/>
       <c r="C62" s="20">
         <v>4</v>
       </c>
@@ -2026,8 +2027,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="40"/>
+      <c r="A63" s="33"/>
+      <c r="B63" s="35"/>
       <c r="C63" s="19">
         <v>5</v>
       </c>
@@ -2036,8 +2037,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="40"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="35"/>
       <c r="C64" s="19">
         <v>8</v>
       </c>
@@ -2046,8 +2047,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
-      <c r="B65" s="40"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="35"/>
       <c r="C65" s="19">
         <v>10</v>
       </c>
@@ -2056,8 +2057,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
-      <c r="B66" s="40"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="35"/>
       <c r="C66" s="19">
         <v>12</v>
       </c>
@@ -2066,8 +2067,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
-      <c r="B67" s="40"/>
+      <c r="A67" s="33"/>
+      <c r="B67" s="35"/>
       <c r="C67" s="19">
         <v>13</v>
       </c>
@@ -2076,8 +2077,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
-      <c r="B68" s="40"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="35"/>
       <c r="C68" s="19">
         <v>14</v>
       </c>
@@ -2086,8 +2087,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
-      <c r="B69" s="40"/>
+      <c r="A69" s="33"/>
+      <c r="B69" s="35"/>
       <c r="C69" s="19">
         <v>15</v>
       </c>
@@ -2096,8 +2097,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
-      <c r="B70" s="40" t="s">
+      <c r="A70" s="33"/>
+      <c r="B70" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C70" s="20">
@@ -2108,8 +2109,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
-      <c r="B71" s="40"/>
+      <c r="A71" s="33"/>
+      <c r="B71" s="35"/>
       <c r="C71" s="19">
         <v>4</v>
       </c>
@@ -2118,8 +2119,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
-      <c r="B72" s="40"/>
+      <c r="A72" s="33"/>
+      <c r="B72" s="35"/>
       <c r="C72" s="19">
         <v>5</v>
       </c>
@@ -2128,8 +2129,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="44"/>
-      <c r="B73" s="40"/>
+      <c r="A73" s="33"/>
+      <c r="B73" s="35"/>
       <c r="C73" s="19">
         <v>6</v>
       </c>
@@ -2138,8 +2139,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
-      <c r="B74" s="40"/>
+      <c r="A74" s="33"/>
+      <c r="B74" s="35"/>
       <c r="C74" s="20">
         <v>7</v>
       </c>
@@ -2148,8 +2149,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="44"/>
-      <c r="B75" s="40"/>
+      <c r="A75" s="33"/>
+      <c r="B75" s="35"/>
       <c r="C75" s="19">
         <v>8</v>
       </c>
@@ -2158,8 +2159,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
-      <c r="B76" s="40"/>
+      <c r="A76" s="33"/>
+      <c r="B76" s="35"/>
       <c r="C76" s="19">
         <v>10</v>
       </c>
@@ -2168,8 +2169,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
-      <c r="B77" s="40"/>
+      <c r="A77" s="33"/>
+      <c r="B77" s="35"/>
       <c r="C77" s="19">
         <v>11</v>
       </c>
@@ -2178,8 +2179,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="44"/>
-      <c r="B78" s="40"/>
+      <c r="A78" s="33"/>
+      <c r="B78" s="35"/>
       <c r="C78" s="19">
         <v>12</v>
       </c>
@@ -2188,8 +2189,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="44"/>
-      <c r="B79" s="40"/>
+      <c r="A79" s="33"/>
+      <c r="B79" s="35"/>
       <c r="C79" s="19">
         <v>14</v>
       </c>
@@ -2198,7 +2199,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="33"/>
       <c r="B80" s="25" t="s">
         <v>64</v>
       </c>
@@ -2210,8 +2211,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="44"/>
-      <c r="B81" s="40" t="s">
+      <c r="A81" s="33"/>
+      <c r="B81" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C81" s="19">
@@ -2222,8 +2223,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
-      <c r="B82" s="40"/>
+      <c r="A82" s="33"/>
+      <c r="B82" s="35"/>
       <c r="C82" s="19">
         <v>4</v>
       </c>
@@ -2232,8 +2233,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
-      <c r="B83" s="40"/>
+      <c r="A83" s="33"/>
+      <c r="B83" s="35"/>
       <c r="C83" s="19">
         <v>5</v>
       </c>
@@ -2242,8 +2243,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
-      <c r="B84" s="40"/>
+      <c r="A84" s="33"/>
+      <c r="B84" s="35"/>
       <c r="C84" s="19">
         <v>8</v>
       </c>
@@ -2252,8 +2253,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
-      <c r="B85" s="40"/>
+      <c r="A85" s="33"/>
+      <c r="B85" s="35"/>
       <c r="C85" s="19">
         <v>9</v>
       </c>
@@ -2262,8 +2263,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="44"/>
-      <c r="B86" s="40"/>
+      <c r="A86" s="33"/>
+      <c r="B86" s="35"/>
       <c r="C86" s="19">
         <v>10</v>
       </c>
@@ -2272,7 +2273,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
+      <c r="A87" s="33"/>
       <c r="B87" s="27" t="s">
         <v>35</v>
       </c>
@@ -2284,10 +2285,10 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="43" t="s">
+      <c r="A88" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B88" s="40" t="s">
+      <c r="B88" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C88" s="20">
@@ -2298,8 +2299,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
-      <c r="B89" s="40"/>
+      <c r="A89" s="33"/>
+      <c r="B89" s="35"/>
       <c r="C89" s="20">
         <v>4</v>
       </c>
@@ -2308,8 +2309,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
-      <c r="B90" s="40"/>
+      <c r="A90" s="33"/>
+      <c r="B90" s="35"/>
       <c r="C90" s="19">
         <v>5</v>
       </c>
@@ -2318,8 +2319,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
-      <c r="B91" s="40"/>
+      <c r="A91" s="33"/>
+      <c r="B91" s="35"/>
       <c r="C91" s="19">
         <v>8</v>
       </c>
@@ -2328,8 +2329,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="40"/>
+      <c r="A92" s="33"/>
+      <c r="B92" s="35"/>
       <c r="C92" s="19">
         <v>10</v>
       </c>
@@ -2338,8 +2339,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
-      <c r="B93" s="40"/>
+      <c r="A93" s="33"/>
+      <c r="B93" s="35"/>
       <c r="C93" s="19">
         <v>12</v>
       </c>
@@ -2348,8 +2349,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
-      <c r="B94" s="40"/>
+      <c r="A94" s="33"/>
+      <c r="B94" s="35"/>
       <c r="C94" s="19">
         <v>13</v>
       </c>
@@ -2358,8 +2359,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
-      <c r="B95" s="40"/>
+      <c r="A95" s="33"/>
+      <c r="B95" s="35"/>
       <c r="C95" s="19">
         <v>14</v>
       </c>
@@ -2368,8 +2369,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="44"/>
-      <c r="B96" s="40"/>
+      <c r="A96" s="33"/>
+      <c r="B96" s="35"/>
       <c r="C96" s="19">
         <v>15</v>
       </c>
@@ -2378,8 +2379,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
-      <c r="B97" s="40" t="s">
+      <c r="A97" s="33"/>
+      <c r="B97" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C97" s="20">
@@ -2390,8 +2391,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
-      <c r="B98" s="40"/>
+      <c r="A98" s="33"/>
+      <c r="B98" s="35"/>
       <c r="C98" s="19">
         <v>4</v>
       </c>
@@ -2400,8 +2401,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="44"/>
-      <c r="B99" s="40"/>
+      <c r="A99" s="33"/>
+      <c r="B99" s="35"/>
       <c r="C99" s="19">
         <v>5</v>
       </c>
@@ -2410,8 +2411,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
-      <c r="B100" s="40"/>
+      <c r="A100" s="33"/>
+      <c r="B100" s="35"/>
       <c r="C100" s="19">
         <v>6</v>
       </c>
@@ -2420,8 +2421,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
-      <c r="B101" s="40"/>
+      <c r="A101" s="33"/>
+      <c r="B101" s="35"/>
       <c r="C101" s="20">
         <v>7</v>
       </c>
@@ -2430,8 +2431,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
-      <c r="B102" s="40"/>
+      <c r="A102" s="33"/>
+      <c r="B102" s="35"/>
       <c r="C102" s="19">
         <v>8</v>
       </c>
@@ -2440,8 +2441,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="44"/>
-      <c r="B103" s="40"/>
+      <c r="A103" s="33"/>
+      <c r="B103" s="35"/>
       <c r="C103" s="19">
         <v>10</v>
       </c>
@@ -2450,8 +2451,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="44"/>
-      <c r="B104" s="40"/>
+      <c r="A104" s="33"/>
+      <c r="B104" s="35"/>
       <c r="C104" s="19">
         <v>11</v>
       </c>
@@ -2460,8 +2461,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="44"/>
-      <c r="B105" s="40"/>
+      <c r="A105" s="33"/>
+      <c r="B105" s="35"/>
       <c r="C105" s="19">
         <v>12</v>
       </c>
@@ -2470,8 +2471,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="44"/>
-      <c r="B106" s="40"/>
+      <c r="A106" s="33"/>
+      <c r="B106" s="35"/>
       <c r="C106" s="19">
         <v>14</v>
       </c>
@@ -2480,7 +2481,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="44"/>
+      <c r="A107" s="33"/>
       <c r="B107" s="30" t="s">
         <v>64</v>
       </c>
@@ -2492,8 +2493,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="44"/>
-      <c r="B108" s="40" t="s">
+      <c r="A108" s="33"/>
+      <c r="B108" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C108" s="19">
@@ -2504,8 +2505,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="44"/>
-      <c r="B109" s="40"/>
+      <c r="A109" s="33"/>
+      <c r="B109" s="35"/>
       <c r="C109" s="19">
         <v>4</v>
       </c>
@@ -2514,8 +2515,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="44"/>
-      <c r="B110" s="40"/>
+      <c r="A110" s="33"/>
+      <c r="B110" s="35"/>
       <c r="C110" s="19">
         <v>5</v>
       </c>
@@ -2524,8 +2525,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="44"/>
-      <c r="B111" s="40"/>
+      <c r="A111" s="33"/>
+      <c r="B111" s="35"/>
       <c r="C111" s="19">
         <v>8</v>
       </c>
@@ -2534,8 +2535,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
-      <c r="B112" s="40"/>
+      <c r="A112" s="33"/>
+      <c r="B112" s="35"/>
       <c r="C112" s="19">
         <v>9</v>
       </c>
@@ -2544,8 +2545,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="44"/>
-      <c r="B113" s="40"/>
+      <c r="A113" s="33"/>
+      <c r="B113" s="35"/>
       <c r="C113" s="19">
         <v>10</v>
       </c>
@@ -2554,7 +2555,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="44"/>
+      <c r="A114" s="33"/>
       <c r="B114" s="31" t="s">
         <v>35</v>
       </c>
@@ -2566,7 +2567,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="41" t="s">
+      <c r="B115" s="36" t="s">
         <v>77</v>
       </c>
       <c r="C115" s="22">
@@ -2577,7 +2578,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="42"/>
+      <c r="B116" s="37"/>
       <c r="C116" s="22">
         <v>6</v>
       </c>
@@ -2586,7 +2587,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="42"/>
+      <c r="B117" s="37"/>
       <c r="C117" s="22">
         <v>7</v>
       </c>
@@ -2596,27 +2597,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B51:B60"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="B33:B42"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B61:B69"/>
+    <mergeCell ref="B70:B79"/>
+    <mergeCell ref="B81:B86"/>
     <mergeCell ref="A24:A60"/>
     <mergeCell ref="A61:A87"/>
     <mergeCell ref="A88:A114"/>
     <mergeCell ref="B88:B96"/>
     <mergeCell ref="B97:B106"/>
     <mergeCell ref="B108:B113"/>
-    <mergeCell ref="B115:B117"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B61:B69"/>
-    <mergeCell ref="B70:B79"/>
-    <mergeCell ref="B81:B86"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B50:B59"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="B33:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>